<commit_message>
[EDIT] export user code
</commit_message>
<xml_diff>
--- a/pabi_security/xlsx_template/xlsx_report_assign_security.xlsx
+++ b/pabi_security/xlsx_template/xlsx_report_assign_security.xlsx
@@ -170,7 +170,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -217,12 +217,6 @@
       <name val="arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -279,13 +273,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -293,11 +291,11 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -305,13 +303,17 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -325,10 +327,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -356,12 +354,12 @@
   <dimension ref="A1:AO12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12:AO12"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.89"/>
@@ -376,221 +374,225 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2"/>
+      <c r="A1" s="2"/>
+      <c r="B1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5"/>
+      <c r="B3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="5"/>
+      <c r="B4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="7"/>
+      <c r="B5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="7"/>
+      <c r="B6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="8"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="10"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="8"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="8"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="8"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="10"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="9"/>
-      <c r="B11" s="10" t="s">
+      <c r="A11" s="11"/>
+      <c r="B11" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G11" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="H11" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="10" t="s">
+      <c r="I11" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="10" t="s">
+      <c r="J11" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="K11" s="10" t="s">
+      <c r="K11" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="L11" s="11" t="s">
+      <c r="L11" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="M11" s="11" t="s">
+      <c r="M11" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="N11" s="11" t="s">
+      <c r="N11" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="O11" s="11" t="s">
+      <c r="O11" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="P11" s="11" t="s">
+      <c r="P11" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="Q11" s="11" t="s">
+      <c r="Q11" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="R11" s="11" t="s">
+      <c r="R11" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="S11" s="11" t="s">
+      <c r="S11" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="T11" s="11" t="s">
+      <c r="T11" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="U11" s="11" t="s">
+      <c r="U11" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="V11" s="12" t="s">
+      <c r="V11" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="W11" s="12" t="s">
+      <c r="W11" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="X11" s="12" t="s">
+      <c r="X11" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="Y11" s="12" t="s">
+      <c r="Y11" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="Z11" s="12" t="s">
+      <c r="Z11" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="AA11" s="12" t="s">
+      <c r="AA11" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="AB11" s="12" t="s">
+      <c r="AB11" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="AC11" s="12" t="s">
+      <c r="AC11" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="AD11" s="12" t="s">
+      <c r="AD11" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="AE11" s="12" t="s">
+      <c r="AE11" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="AF11" s="12" t="s">
+      <c r="AF11" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="AG11" s="12" t="s">
+      <c r="AG11" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="AH11" s="12" t="s">
+      <c r="AH11" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="AI11" s="12" t="s">
+      <c r="AI11" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="AJ11" s="12" t="s">
+      <c r="AJ11" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="AK11" s="12" t="s">
+      <c r="AK11" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="AL11" s="12" t="s">
+      <c r="AL11" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="AM11" s="12" t="s">
+      <c r="AM11" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="AN11" s="12" t="s">
+      <c r="AN11" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="AO11" s="12" t="s">
+      <c r="AO11" s="13" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
-      <c r="N12" s="11"/>
-      <c r="O12" s="11"/>
-      <c r="P12" s="11"/>
-      <c r="Q12" s="11"/>
-      <c r="R12" s="11"/>
-      <c r="S12" s="11"/>
-      <c r="T12" s="11"/>
-      <c r="U12" s="11"/>
-      <c r="V12" s="11"/>
-      <c r="W12" s="11"/>
-      <c r="X12" s="11"/>
-      <c r="Y12" s="11"/>
-      <c r="Z12" s="11"/>
-      <c r="AA12" s="11"/>
-      <c r="AB12" s="11"/>
-      <c r="AC12" s="11"/>
-      <c r="AD12" s="11"/>
-      <c r="AE12" s="11"/>
-      <c r="AF12" s="11"/>
-      <c r="AG12" s="11"/>
-      <c r="AH12" s="11"/>
-      <c r="AI12" s="11" t="s">
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
+      <c r="P12" s="13"/>
+      <c r="Q12" s="13"/>
+      <c r="R12" s="13"/>
+      <c r="S12" s="13"/>
+      <c r="T12" s="13"/>
+      <c r="U12" s="13"/>
+      <c r="V12" s="13"/>
+      <c r="W12" s="13"/>
+      <c r="X12" s="13"/>
+      <c r="Y12" s="13"/>
+      <c r="Z12" s="13"/>
+      <c r="AA12" s="13"/>
+      <c r="AB12" s="13"/>
+      <c r="AC12" s="13"/>
+      <c r="AD12" s="13"/>
+      <c r="AE12" s="13"/>
+      <c r="AF12" s="13"/>
+      <c r="AG12" s="13"/>
+      <c r="AH12" s="13"/>
+      <c r="AI12" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="AJ12" s="11"/>
-      <c r="AK12" s="11" t="s">
+      <c r="AJ12" s="13"/>
+      <c r="AK12" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="AL12" s="11"/>
-      <c r="AM12" s="11"/>
-      <c r="AN12" s="11"/>
-      <c r="AO12" s="11"/>
+      <c r="AL12" s="13"/>
+      <c r="AM12" s="13"/>
+      <c r="AN12" s="13"/>
+      <c r="AO12" s="13"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>